<commit_message>
Import and validate inventory workbook with swing
</commit_message>
<xml_diff>
--- a/src/Files/InvalidWorkbook.xlsx
+++ b/src/Files/InvalidWorkbook.xlsx
@@ -16,10 +16,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
   <si>
-    <t>This is an invalid workbook</t>
+    <t>test</t>
   </si>
   <si>
-    <t>test</t>
+    <t>inventory work book</t>
   </si>
 </sst>
 </file>
@@ -379,29 +379,29 @@
   <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.55000000000000004">

</xml_diff>